<commit_message>
header of report and data dictionary
</commit_message>
<xml_diff>
--- a/dic/dictionary.xlsx
+++ b/dic/dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sopheap/Desktop/R/AMS/dic/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sopheap/Desktop/R/AMC/dic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8FE1334-4770-3B40-8EA5-D82735D16143}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C536A8D2-3E76-6D48-9BA8-E190B9544153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="500" windowWidth="27580" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1220" yWindow="500" windowWidth="27580" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dict" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="128">
   <si>
     <t>commodity_name</t>
   </si>
@@ -401,12 +401,33 @@
   </si>
   <si>
     <t>PO</t>
+  </si>
+  <si>
+    <t>Start date</t>
+  </si>
+  <si>
+    <t>End date</t>
+  </si>
+  <si>
+    <t>parameter</t>
+  </si>
+  <si>
+    <t>Hospital</t>
+  </si>
+  <si>
+    <t>report</t>
+  </si>
+  <si>
+    <t>Siem Reap Provincial Referral  Hospital</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd\-mm\-yy"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -448,7 +469,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -464,6 +485,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -506,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -541,6 +568,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -840,7 +873,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScale="159" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1741,10 +1774,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F185A0-60D8-1245-8925-D9DD2909F606}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1753,10 +1786,13 @@
     <col min="2" max="2" width="17.5" style="11" customWidth="1"/>
     <col min="3" max="3" width="14.6640625" style="10" customWidth="1"/>
     <col min="4" max="4" width="16.5" style="10" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="10"/>
+    <col min="5" max="5" width="10.83203125" style="10"/>
+    <col min="6" max="6" width="14" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.83203125" style="10" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>110</v>
       </c>
@@ -1769,8 +1805,14 @@
       <c r="D1" s="6" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F1" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>96</v>
       </c>
@@ -1783,8 +1825,14 @@
       <c r="D2" s="5">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F2" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="G2" s="16">
+        <v>43466</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>97</v>
       </c>
@@ -1797,8 +1845,14 @@
       <c r="D3" s="5">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F3" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="16">
+        <v>43830</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>98</v>
       </c>
@@ -1811,8 +1865,14 @@
       <c r="D4" s="5">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F4" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>99</v>
       </c>
@@ -1826,7 +1886,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>100</v>
       </c>
@@ -1840,7 +1900,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>117</v>
       </c>
@@ -1854,7 +1914,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>118</v>
       </c>
@@ -1868,7 +1928,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>101</v>
       </c>
@@ -1882,7 +1942,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>102</v>
       </c>
@@ -1896,7 +1956,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>103</v>
       </c>
@@ -1910,7 +1970,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>104</v>
       </c>
@@ -1924,7 +1984,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>105</v>
       </c>
@@ -1938,7 +1998,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>106</v>
       </c>
@@ -1956,6 +2016,10 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="dd-mm-yy" promptTitle="information" prompt="dd-mm-yy" sqref="G3" xr:uid="{9BA3D6EF-5D9E-AA49-AB85-28C6BED18EF1}"/>
+    <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="information" prompt="dd-mm-yy" sqref="G2" xr:uid="{87DCF04F-C4F3-B14C-847B-63ADCA91088A}"/>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
calculate quarterly instead of monthly
</commit_message>
<xml_diff>
--- a/dic/dictionary.xlsx
+++ b/dic/dictionary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sopheap/Desktop/R/AMC/dic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C536A8D2-3E76-6D48-9BA8-E190B9544153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9606A1-9B5A-C44C-BC2A-0EB4B3F476B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1220" yWindow="500" windowWidth="27580" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -533,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -575,6 +575,8 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1774,10 +1776,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F185A0-60D8-1245-8925-D9DD2909F606}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1789,10 +1791,13 @@
     <col min="5" max="5" width="10.83203125" style="10"/>
     <col min="6" max="6" width="14" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.83203125" style="10" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="10"/>
+    <col min="8" max="8" width="10.83203125" style="10"/>
+    <col min="9" max="9" width="15" style="10" customWidth="1"/>
+    <col min="10" max="10" width="16.1640625" style="10" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>110</v>
       </c>
@@ -1812,7 +1817,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
         <v>96</v>
       </c>
@@ -1831,8 +1836,10 @@
       <c r="G2" s="16">
         <v>43466</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I2" s="18"/>
+      <c r="J2" s="17"/>
+    </row>
+    <row r="3" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>97</v>
       </c>
@@ -1852,7 +1859,7 @@
         <v>43830</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>98</v>
       </c>
@@ -1872,7 +1879,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>99</v>
       </c>
@@ -1886,7 +1893,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>100</v>
       </c>
@@ -1900,7 +1907,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>117</v>
       </c>
@@ -1914,7 +1921,7 @@
         <v>5.2</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>118</v>
       </c>
@@ -1928,7 +1935,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>101</v>
       </c>
@@ -1942,7 +1949,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>102</v>
       </c>
@@ -1956,7 +1963,7 @@
         <v>4.7</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>103</v>
       </c>
@@ -1970,7 +1977,7 @@
         <v>5.4</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>104</v>
       </c>
@@ -1984,7 +1991,7 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="26" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>105</v>
       </c>
@@ -1998,7 +2005,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>106</v>
       </c>

</xml_diff>

<commit_message>
update to be automate
</commit_message>
<xml_diff>
--- a/dic/dictionary.xlsx
+++ b/dic/dictionary.xlsx
@@ -5,19 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sopheap/Desktop/R/AMC 3 Nov 21 DK/dic/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sopheap/Desktop/R/AMC/dic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B50A032-7CB9-1D43-8613-7A68DBDD47E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{092A09C1-0F7A-D94B-9B6D-7497899883C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="500" windowWidth="27520" windowHeight="16700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hospital" sheetId="2" r:id="rId1"/>
     <sheet name="Dict" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Dict!$B$1:$H$64</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Dict!$A$1:$H$64</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="131">
   <si>
     <t>AMC</t>
   </si>
@@ -208,9 +208,6 @@
     <t>3.6</t>
   </si>
   <si>
-    <t>BNB</t>
-  </si>
-  <si>
     <t>PEN</t>
   </si>
   <si>
@@ -412,22 +409,25 @@
     <t>Penicilline G</t>
   </si>
   <si>
+    <t>Trimethoprim/sulfamethoxazole</t>
+  </si>
+  <si>
+    <t>Tetracycline</t>
+  </si>
+  <si>
+    <t>Vancomycin</t>
+  </si>
+  <si>
+    <t>full_name</t>
+  </si>
+  <si>
     <t>Phenoxymethylpenicillin</t>
   </si>
   <si>
-    <t>Trimethoprim/sulfamethoxazole</t>
-  </si>
-  <si>
-    <t>Tetracycline</t>
-  </si>
-  <si>
-    <t>Vancomycin</t>
-  </si>
-  <si>
-    <t>full_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Takeo hospital </t>
+    <t>BNP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siem Reap hospital </t>
   </si>
 </sst>
 </file>
@@ -857,7 +857,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -872,15 +872,15 @@
   <sheetData>
     <row r="1" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="10">
         <v>43831</v>
@@ -890,15 +890,15 @@
     </row>
     <row r="3" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B3" s="10">
-        <v>44135</v>
+        <v>44196</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>130</v>
@@ -924,13 +924,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H64"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C31" sqref="C31"/>
+      <selection pane="bottomRight" activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -945,16 +946,16 @@
   <sheetData>
     <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>23</v>
@@ -966,19 +967,19 @@
         <v>50</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>36</v>
@@ -991,16 +992,16 @@
       </c>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>24</v>
@@ -1012,19 +1013,19 @@
         <v>1.5</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>35</v>
@@ -1036,19 +1037,19 @@
         <v>1</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>25</v>
@@ -1060,19 +1061,19 @@
         <v>1</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>25</v>
@@ -1084,19 +1085,19 @@
         <v>2</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>31</v>
@@ -1108,19 +1109,19 @@
         <v>6</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>25</v>
@@ -1132,19 +1133,19 @@
         <v>53</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>26</v>
@@ -1156,12 +1157,12 @@
         <v>53</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>1</v>
@@ -1170,10 +1171,10 @@
         <v>33</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F10" s="4">
         <v>2.5</v>
@@ -1182,24 +1183,24 @@
         <v>1.5</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F11" s="4">
         <v>1.5</v>
@@ -1208,19 +1209,19 @@
         <v>1.5</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>26</v>
@@ -1232,19 +1233,19 @@
         <v>54</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>25</v>
@@ -1256,19 +1257,19 @@
         <v>54</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>57</v>
+        <v>129</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>37</v>
@@ -1280,19 +1281,19 @@
         <v>3.6</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>31</v>
@@ -1304,19 +1305,19 @@
         <v>4</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>26</v>
@@ -1328,19 +1329,19 @@
         <v>1</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>30</v>
@@ -1352,19 +1353,19 @@
         <v>0.4</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>48</v>
@@ -1376,19 +1377,19 @@
         <v>49</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>31</v>
@@ -1400,19 +1401,19 @@
         <v>3</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>25</v>
@@ -1424,19 +1425,19 @@
         <v>1</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>26</v>
@@ -1448,19 +1449,19 @@
         <v>1</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>30</v>
@@ -1472,19 +1473,19 @@
         <v>0.8</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>26</v>
@@ -1496,19 +1497,19 @@
         <v>2</v>
       </c>
       <c r="H23" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>25</v>
@@ -1520,19 +1521,19 @@
         <v>2</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>31</v>
@@ -1544,19 +1545,19 @@
         <v>2</v>
       </c>
       <c r="H25" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>25</v>
@@ -1568,19 +1569,19 @@
         <v>0.5</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>31</v>
@@ -1592,19 +1593,19 @@
         <v>2</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>31</v>
@@ -1616,22 +1617,22 @@
         <v>4</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F29" s="4">
         <v>0.75</v>
@@ -1640,19 +1641,19 @@
         <v>3</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>31</v>
@@ -1664,19 +1665,19 @@
         <v>3</v>
       </c>
       <c r="H30" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>28</v>
@@ -1688,19 +1689,19 @@
         <v>55</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>26</v>
@@ -1712,19 +1713,19 @@
         <v>2</v>
       </c>
       <c r="H32" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>25</v>
@@ -1736,24 +1737,24 @@
         <v>2</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F34" s="4">
         <v>1.5</v>
@@ -1762,19 +1763,19 @@
         <v>2</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>31</v>
@@ -1786,19 +1787,19 @@
         <v>4</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>28</v>
@@ -1811,16 +1812,16 @@
       </c>
       <c r="H36" s="7"/>
     </row>
-    <row r="37" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>30</v>
@@ -1833,16 +1834,16 @@
       </c>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C38" s="3"/>
       <c r="D38" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>32</v>
@@ -1854,19 +1855,19 @@
         <v>52</v>
       </c>
       <c r="H38" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>28</v>
@@ -1878,19 +1879,19 @@
         <v>0.5</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>26</v>
@@ -1902,22 +1903,22 @@
         <v>0.5</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F41" s="4">
         <v>0.5</v>
@@ -1926,19 +1927,19 @@
         <v>0.5</v>
       </c>
       <c r="H41" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>31</v>
@@ -1950,19 +1951,19 @@
         <v>3</v>
       </c>
       <c r="H42" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>25</v>
@@ -1974,19 +1975,19 @@
         <v>3</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>48</v>
@@ -1998,19 +1999,19 @@
         <v>0.4</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>26</v>
@@ -2022,21 +2023,19 @@
         <v>53</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C46" s="3" t="s">
-        <v>33</v>
-      </c>
+      <c r="C46" s="3"/>
       <c r="D46" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>33</v>
@@ -2048,46 +2047,48 @@
         <v>53</v>
       </c>
       <c r="H46" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C47" s="3"/>
+      <c r="C47" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="D47" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="F47" s="4">
+        <v>0.5</v>
       </c>
       <c r="G47" s="4" t="s">
         <v>53</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B48" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C48" s="14"/>
       <c r="D48" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F48" s="15">
         <v>2.4</v>
@@ -2096,19 +2097,19 @@
         <v>1.5</v>
       </c>
       <c r="H48" s="16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>25</v>
@@ -2120,19 +2121,19 @@
         <v>4</v>
       </c>
       <c r="H49" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C50" s="3"/>
       <c r="D50" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>28</v>
@@ -2144,19 +2145,19 @@
         <v>0.2</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" s="17" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" s="17" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B51" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>29</v>
@@ -2169,16 +2170,16 @@
       </c>
       <c r="H51" s="7"/>
     </row>
-    <row r="52" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C52" s="3"/>
       <c r="D52" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>30</v>
@@ -2190,19 +2191,19 @@
         <v>0.4</v>
       </c>
       <c r="H52" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>34</v>
@@ -2214,19 +2215,19 @@
         <v>56</v>
       </c>
       <c r="H53" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>26</v>
@@ -2238,22 +2239,22 @@
         <v>2</v>
       </c>
       <c r="H54" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F55" s="4">
         <v>0.48</v>
@@ -2262,22 +2263,22 @@
         <v>4</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C56" s="3"/>
       <c r="D56" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F56" s="4">
         <v>0.96</v>
@@ -2286,12 +2287,12 @@
         <v>4</v>
       </c>
       <c r="H56" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>5</v>
@@ -2300,10 +2301,10 @@
         <v>33</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F57" s="4">
         <v>4.8</v>
@@ -2312,19 +2313,19 @@
         <v>4</v>
       </c>
       <c r="H57" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C58" s="3"/>
       <c r="D58" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>27</v>
@@ -2336,22 +2337,22 @@
         <v>4</v>
       </c>
       <c r="H58" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C59" s="3"/>
       <c r="D59" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F59" s="4">
         <v>0.12</v>
@@ -2360,22 +2361,22 @@
         <v>4</v>
       </c>
       <c r="H59" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C60" s="3"/>
       <c r="D60" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F60" s="4">
         <v>0.96</v>
@@ -2384,24 +2385,24 @@
         <v>4</v>
       </c>
       <c r="H60" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F61" s="4">
         <v>2.88</v>
@@ -2410,24 +2411,24 @@
         <v>4</v>
       </c>
       <c r="H61" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F62" s="4">
         <v>2.4</v>
@@ -2436,19 +2437,19 @@
         <v>4</v>
       </c>
       <c r="H62" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C63" s="3"/>
       <c r="D63" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>26</v>
@@ -2460,19 +2461,19 @@
         <v>1</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C64" s="3"/>
       <c r="D64" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>31</v>
@@ -2484,10 +2485,17 @@
         <v>2</v>
       </c>
       <c r="H64" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H64" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Amikacin"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>